<commit_message>
created test cases for email verification api
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_40.xlsx
+++ b/test_case_report/sprint_40.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33600C05-D0D6-40F8-9AE9-77695A849630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE26881-6352-4F3F-842F-95856480F460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:C57"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -584,19 +584,25 @@
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>2000</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="18.75">
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>1294</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="18.75">
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5">
+        <v>755</v>
+      </c>
     </row>
     <row r="14" spans="2:3" ht="18.75" customHeight="1">
       <c r="B14" s="6" t="s">
@@ -792,16 +798,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
created api test cases for reset pass
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_40.xlsx
+++ b/test_case_report/sprint_40.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE26881-6352-4F3F-842F-95856480F460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE3E1E1-7EA8-4AEB-B97D-29BA543DE925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -614,19 +614,25 @@
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>2178</v>
+      </c>
     </row>
     <row r="16" spans="2:3" ht="18.75">
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>1294</v>
+      </c>
     </row>
     <row r="17" spans="2:3" ht="18.75">
       <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>755</v>
+      </c>
     </row>
     <row r="20" spans="2:3" ht="18.75">
       <c r="B20" s="6" t="s">
@@ -638,19 +644,25 @@
       <c r="B21" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2">
+        <v>2360</v>
+      </c>
     </row>
     <row r="22" spans="2:3" ht="18.75">
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4">
+        <v>1294</v>
+      </c>
     </row>
     <row r="23" spans="2:3" ht="18.75">
       <c r="B23" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="5">
+        <v>755</v>
+      </c>
     </row>
     <row r="26" spans="2:3" ht="18.75">
       <c r="B26" s="6" t="s">

</xml_diff>

<commit_message>
created api test cases for login device type pos+neg,fibmesh step-2 signup
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_40.xlsx
+++ b/test_case_report/sprint_40.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC20797-7545-43D4-805B-E504207DDB90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AEC663-13C4-4E45-A0BC-FDBCD5FF6E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -734,19 +734,25 @@
       <c r="B39" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2">
+        <v>2829</v>
+      </c>
     </row>
     <row r="40" spans="2:3" ht="18.75">
       <c r="B40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="4"/>
+      <c r="C40" s="4">
+        <v>1367</v>
+      </c>
     </row>
     <row r="41" spans="2:3" ht="18.75">
       <c r="B41" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="5"/>
+      <c r="C41" s="5">
+        <v>803</v>
+      </c>
     </row>
     <row r="44" spans="2:3" ht="18.75">
       <c r="B44" s="6" t="s">
@@ -822,16 +828,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>